<commit_message>
added test user for devs
</commit_message>
<xml_diff>
--- a/test/fixtures/consolidated-users.xlsx
+++ b/test/fixtures/consolidated-users.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27420" yWindow="2280" windowWidth="29820" windowHeight="16120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4676" uniqueCount="2393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4682" uniqueCount="2395">
   <si>
     <t>Email</t>
   </si>
@@ -7221,6 +7221,12 @@
   </si>
   <si>
     <t>sarahrp20@yahoo.com</t>
+  </si>
+  <si>
+    <t>admin@test.com</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -7916,8 +7922,8 @@
   <dimension ref="A1:I523"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
+      <pane ySplit="1" topLeftCell="A490" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A517" sqref="A517"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -22485,6 +22491,24 @@
       <c r="I517" s="18"/>
     </row>
     <row r="518" spans="1:9">
+      <c r="A518" s="61" t="s">
+        <v>2393</v>
+      </c>
+      <c r="B518" s="18" t="s">
+        <v>2394</v>
+      </c>
+      <c r="C518" s="18" t="s">
+        <v>2338</v>
+      </c>
+      <c r="D518" t="s">
+        <v>2394</v>
+      </c>
+      <c r="E518" t="s">
+        <v>2394</v>
+      </c>
+      <c r="F518" s="47" t="s">
+        <v>2341</v>
+      </c>
       <c r="G518"/>
     </row>
     <row r="519" spans="1:9">
@@ -22827,6 +22851,7 @@
     <hyperlink ref="A6" r:id="rId318"/>
     <hyperlink ref="A7" r:id="rId319"/>
     <hyperlink ref="A122" r:id="rId320"/>
+    <hyperlink ref="A518" r:id="rId321"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>